<commit_message>
fix typo/spacing; use materials_combined
</commit_message>
<xml_diff>
--- a/data/raw_data - Copy.xlsx
+++ b/data/raw_data - Copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\paktulay-doors\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75FEC73-395F-47CE-8C61-8F8DD6D76E84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8673F7E-97E7-4753-B3EF-C459D21BD73F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{F3A75742-B43B-409A-9361-00192F1802B9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{F3A75742-B43B-409A-9361-00192F1802B9}"/>
   </bookViews>
   <sheets>
     <sheet name="tinggi lebar" sheetId="1" r:id="rId1"/>
@@ -253,9 +253,6 @@
     <t>M4''</t>
   </si>
   <si>
-    <t>M4''+ TUTUP GOT</t>
-  </si>
-  <si>
     <t>M4'' + TUTUP M</t>
   </si>
   <si>
@@ -314,6 +311,9 @@
   </si>
   <si>
     <t>OB4'' + TUTUP M + BELL BAWAH</t>
+  </si>
+  <si>
+    <t>M4'' + TUTUP GOT</t>
   </si>
 </sst>
 </file>
@@ -688,11 +688,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13074309-71A8-4105-A964-6E8ADE1034BF}">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K1" sqref="K1"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,7 +743,7 @@
         <v>66</v>
       </c>
       <c r="L1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -1728,7 +1728,7 @@
         <v>66</v>
       </c>
       <c r="U1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
@@ -2964,11 +2964,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8D5488C-3F40-4C0C-9DBF-344688341C49}">
   <dimension ref="A1:U34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3058,7 +3058,7 @@
         <v>66</v>
       </c>
       <c r="U1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
@@ -3149,7 +3149,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="E6" t="s">
         <v>69</v>
@@ -3158,22 +3158,22 @@
         <v>69</v>
       </c>
       <c r="M6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P6" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>78</v>
+      </c>
+      <c r="R6" t="s">
         <v>80</v>
       </c>
-      <c r="Q6" t="s">
-        <v>79</v>
-      </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>81</v>
-      </c>
-      <c r="S6" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -3181,31 +3181,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="E7" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="G7" t="s">
         <v>69</v>
       </c>
       <c r="M7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P7" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>78</v>
+      </c>
+      <c r="R7" t="s">
         <v>80</v>
       </c>
-      <c r="Q7" t="s">
-        <v>79</v>
-      </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>81</v>
-      </c>
-      <c r="S7" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
@@ -3213,31 +3213,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="G8" t="s">
         <v>69</v>
       </c>
       <c r="M8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P8" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>78</v>
+      </c>
+      <c r="R8" t="s">
         <v>80</v>
       </c>
-      <c r="Q8" t="s">
-        <v>79</v>
-      </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>81</v>
-      </c>
-      <c r="S8" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
@@ -3245,31 +3245,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="E9" t="s">
         <v>69</v>
       </c>
       <c r="G9" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="M9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P9" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>78</v>
+      </c>
+      <c r="R9" t="s">
         <v>80</v>
       </c>
-      <c r="Q9" t="s">
-        <v>79</v>
-      </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>81</v>
-      </c>
-      <c r="S9" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
@@ -3277,31 +3277,31 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="E10" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="G10" t="s">
         <v>69</v>
       </c>
       <c r="M10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P10" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>78</v>
+      </c>
+      <c r="R10" t="s">
         <v>80</v>
       </c>
-      <c r="Q10" t="s">
-        <v>79</v>
-      </c>
-      <c r="R10" t="s">
+      <c r="S10" t="s">
         <v>81</v>
-      </c>
-      <c r="S10" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
@@ -3309,31 +3309,31 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="E11" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="G11" t="s">
         <v>69</v>
       </c>
       <c r="M11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P11" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>78</v>
+      </c>
+      <c r="R11" t="s">
         <v>80</v>
       </c>
-      <c r="Q11" t="s">
-        <v>79</v>
-      </c>
-      <c r="R11" t="s">
+      <c r="S11" t="s">
         <v>81</v>
-      </c>
-      <c r="S11" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
@@ -3341,37 +3341,37 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="E12" t="s">
         <v>69</v>
       </c>
       <c r="F12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G12" t="s">
         <v>69</v>
       </c>
       <c r="M12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P12" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>78</v>
+      </c>
+      <c r="R12" t="s">
         <v>80</v>
       </c>
-      <c r="Q12" t="s">
-        <v>79</v>
-      </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>81</v>
       </c>
-      <c r="S12" t="s">
-        <v>82</v>
-      </c>
       <c r="U12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
@@ -3379,37 +3379,37 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="E13" t="s">
         <v>69</v>
       </c>
       <c r="F13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G13" t="s">
         <v>69</v>
       </c>
       <c r="M13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P13" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>78</v>
+      </c>
+      <c r="R13" t="s">
         <v>80</v>
       </c>
-      <c r="Q13" t="s">
-        <v>79</v>
-      </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>81</v>
       </c>
-      <c r="S13" t="s">
-        <v>82</v>
-      </c>
       <c r="U13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
@@ -3417,37 +3417,37 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" t="s">
         <v>70</v>
-      </c>
-      <c r="E14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F14" t="s">
-        <v>71</v>
       </c>
       <c r="G14" t="s">
         <v>69</v>
       </c>
       <c r="M14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P14" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>78</v>
+      </c>
+      <c r="R14" t="s">
         <v>80</v>
       </c>
-      <c r="Q14" t="s">
-        <v>79</v>
-      </c>
-      <c r="R14" t="s">
+      <c r="S14" t="s">
         <v>81</v>
       </c>
-      <c r="S14" t="s">
-        <v>82</v>
-      </c>
       <c r="U14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
@@ -3455,37 +3455,37 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" t="s">
         <v>70</v>
-      </c>
-      <c r="E15" t="s">
-        <v>70</v>
-      </c>
-      <c r="F15" t="s">
-        <v>71</v>
       </c>
       <c r="G15" t="s">
         <v>69</v>
       </c>
       <c r="M15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P15" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>78</v>
+      </c>
+      <c r="R15" t="s">
         <v>80</v>
       </c>
-      <c r="Q15" t="s">
-        <v>79</v>
-      </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>81</v>
       </c>
-      <c r="S15" t="s">
-        <v>82</v>
-      </c>
       <c r="U15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
@@ -3493,37 +3493,37 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" t="s">
+        <v>82</v>
+      </c>
+      <c r="L16" t="s">
+        <v>79</v>
+      </c>
+      <c r="M16" t="s">
+        <v>78</v>
+      </c>
+      <c r="N16" t="s">
+        <v>85</v>
+      </c>
+      <c r="O16" t="s">
         <v>84</v>
       </c>
-      <c r="E16" t="s">
-        <v>83</v>
-      </c>
-      <c r="G16" t="s">
-        <v>83</v>
-      </c>
-      <c r="L16" t="s">
-        <v>80</v>
-      </c>
-      <c r="M16" t="s">
+      <c r="P16" t="s">
         <v>79</v>
       </c>
-      <c r="N16" t="s">
-        <v>86</v>
-      </c>
-      <c r="O16" t="s">
-        <v>85</v>
-      </c>
-      <c r="P16" t="s">
-        <v>80</v>
-      </c>
       <c r="Q16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S16" s="2"/>
     </row>
@@ -3532,37 +3532,37 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17" t="s">
+        <v>82</v>
+      </c>
+      <c r="L17" t="s">
+        <v>79</v>
+      </c>
+      <c r="M17" t="s">
+        <v>78</v>
+      </c>
+      <c r="N17" t="s">
+        <v>85</v>
+      </c>
+      <c r="O17" t="s">
         <v>84</v>
       </c>
-      <c r="E17" t="s">
-        <v>83</v>
-      </c>
-      <c r="G17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L17" t="s">
-        <v>80</v>
-      </c>
-      <c r="M17" t="s">
+      <c r="P17" t="s">
         <v>79</v>
       </c>
-      <c r="N17" t="s">
-        <v>86</v>
-      </c>
-      <c r="O17" t="s">
-        <v>85</v>
-      </c>
-      <c r="P17" t="s">
-        <v>80</v>
-      </c>
       <c r="Q17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S17" s="2"/>
     </row>
@@ -3571,37 +3571,37 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" t="s">
+        <v>82</v>
+      </c>
+      <c r="L18" t="s">
+        <v>79</v>
+      </c>
+      <c r="M18" t="s">
+        <v>78</v>
+      </c>
+      <c r="N18" t="s">
+        <v>85</v>
+      </c>
+      <c r="O18" t="s">
         <v>84</v>
       </c>
-      <c r="E18" t="s">
-        <v>83</v>
-      </c>
-      <c r="G18" t="s">
-        <v>83</v>
-      </c>
-      <c r="L18" t="s">
-        <v>80</v>
-      </c>
-      <c r="M18" t="s">
+      <c r="P18" t="s">
         <v>79</v>
       </c>
-      <c r="N18" t="s">
-        <v>86</v>
-      </c>
-      <c r="O18" t="s">
-        <v>85</v>
-      </c>
-      <c r="P18" t="s">
-        <v>80</v>
-      </c>
       <c r="Q18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S18" s="2"/>
     </row>
@@ -3610,37 +3610,37 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G19" t="s">
+        <v>82</v>
+      </c>
+      <c r="L19" t="s">
+        <v>79</v>
+      </c>
+      <c r="M19" t="s">
+        <v>78</v>
+      </c>
+      <c r="N19" t="s">
+        <v>85</v>
+      </c>
+      <c r="O19" t="s">
         <v>84</v>
       </c>
-      <c r="E19" t="s">
-        <v>83</v>
-      </c>
-      <c r="G19" t="s">
-        <v>83</v>
-      </c>
-      <c r="L19" t="s">
-        <v>80</v>
-      </c>
-      <c r="M19" t="s">
+      <c r="P19" t="s">
         <v>79</v>
       </c>
-      <c r="N19" t="s">
-        <v>86</v>
-      </c>
-      <c r="O19" t="s">
-        <v>85</v>
-      </c>
-      <c r="P19" t="s">
-        <v>80</v>
-      </c>
       <c r="Q19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S19" s="2"/>
     </row>
@@ -3649,37 +3649,37 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" t="s">
+        <v>82</v>
+      </c>
+      <c r="L20" t="s">
+        <v>79</v>
+      </c>
+      <c r="M20" t="s">
+        <v>78</v>
+      </c>
+      <c r="N20" t="s">
+        <v>85</v>
+      </c>
+      <c r="O20" t="s">
         <v>84</v>
       </c>
-      <c r="E20" t="s">
-        <v>83</v>
-      </c>
-      <c r="G20" t="s">
-        <v>83</v>
-      </c>
-      <c r="L20" t="s">
-        <v>80</v>
-      </c>
-      <c r="M20" t="s">
+      <c r="P20" t="s">
         <v>79</v>
       </c>
-      <c r="N20" t="s">
-        <v>86</v>
-      </c>
-      <c r="O20" t="s">
-        <v>85</v>
-      </c>
-      <c r="P20" t="s">
-        <v>80</v>
-      </c>
       <c r="Q20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S20" s="2"/>
     </row>
@@ -3688,37 +3688,37 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D21" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" t="s">
+        <v>82</v>
+      </c>
+      <c r="G21" t="s">
+        <v>82</v>
+      </c>
+      <c r="L21" t="s">
+        <v>79</v>
+      </c>
+      <c r="M21" t="s">
+        <v>78</v>
+      </c>
+      <c r="N21" t="s">
+        <v>85</v>
+      </c>
+      <c r="O21" t="s">
         <v>84</v>
       </c>
-      <c r="E21" t="s">
-        <v>83</v>
-      </c>
-      <c r="G21" t="s">
-        <v>83</v>
-      </c>
-      <c r="L21" t="s">
-        <v>80</v>
-      </c>
-      <c r="M21" t="s">
+      <c r="P21" t="s">
         <v>79</v>
       </c>
-      <c r="N21" t="s">
-        <v>86</v>
-      </c>
-      <c r="O21" t="s">
-        <v>85</v>
-      </c>
-      <c r="P21" t="s">
-        <v>80</v>
-      </c>
       <c r="Q21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S21" s="2"/>
     </row>
@@ -3727,37 +3727,37 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D22" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" t="s">
+        <v>82</v>
+      </c>
+      <c r="G22" t="s">
+        <v>82</v>
+      </c>
+      <c r="L22" t="s">
+        <v>79</v>
+      </c>
+      <c r="M22" t="s">
+        <v>78</v>
+      </c>
+      <c r="N22" t="s">
+        <v>85</v>
+      </c>
+      <c r="O22" t="s">
         <v>84</v>
       </c>
-      <c r="E22" t="s">
-        <v>83</v>
-      </c>
-      <c r="G22" t="s">
-        <v>83</v>
-      </c>
-      <c r="L22" t="s">
-        <v>80</v>
-      </c>
-      <c r="M22" t="s">
+      <c r="P22" t="s">
         <v>79</v>
       </c>
-      <c r="N22" t="s">
-        <v>86</v>
-      </c>
-      <c r="O22" t="s">
-        <v>85</v>
-      </c>
-      <c r="P22" t="s">
-        <v>80</v>
-      </c>
       <c r="Q22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S22" s="2"/>
     </row>
@@ -3766,37 +3766,37 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" t="s">
+        <v>82</v>
+      </c>
+      <c r="G23" t="s">
+        <v>82</v>
+      </c>
+      <c r="L23" t="s">
+        <v>79</v>
+      </c>
+      <c r="M23" t="s">
+        <v>78</v>
+      </c>
+      <c r="N23" t="s">
+        <v>85</v>
+      </c>
+      <c r="O23" t="s">
         <v>84</v>
       </c>
-      <c r="E23" t="s">
-        <v>83</v>
-      </c>
-      <c r="G23" t="s">
-        <v>83</v>
-      </c>
-      <c r="L23" t="s">
-        <v>80</v>
-      </c>
-      <c r="M23" t="s">
+      <c r="P23" t="s">
         <v>79</v>
       </c>
-      <c r="N23" t="s">
-        <v>86</v>
-      </c>
-      <c r="O23" t="s">
-        <v>85</v>
-      </c>
-      <c r="P23" t="s">
-        <v>80</v>
-      </c>
       <c r="Q23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S23" s="2"/>
     </row>
@@ -3808,7 +3808,7 @@
         <v>69</v>
       </c>
       <c r="D24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E24" t="s">
         <v>69</v>
@@ -3825,7 +3825,7 @@
         <v>69</v>
       </c>
       <c r="D25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E25" t="s">
         <v>69</v>
@@ -3839,40 +3839,40 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" t="s">
+        <v>82</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D26" t="s">
+      <c r="G26" t="s">
+        <v>82</v>
+      </c>
+      <c r="L26" t="s">
+        <v>79</v>
+      </c>
+      <c r="M26" t="s">
+        <v>78</v>
+      </c>
+      <c r="N26" t="s">
+        <v>85</v>
+      </c>
+      <c r="O26" t="s">
         <v>84</v>
       </c>
-      <c r="E26" t="s">
-        <v>83</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G26" t="s">
-        <v>83</v>
-      </c>
-      <c r="L26" t="s">
-        <v>80</v>
-      </c>
-      <c r="M26" t="s">
+      <c r="P26" t="s">
         <v>79</v>
       </c>
-      <c r="N26" t="s">
-        <v>86</v>
-      </c>
-      <c r="O26" t="s">
-        <v>85</v>
-      </c>
-      <c r="P26" t="s">
-        <v>80</v>
-      </c>
       <c r="Q26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S26" s="2"/>
     </row>
@@ -3881,40 +3881,40 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" t="s">
+        <v>82</v>
+      </c>
+      <c r="F27" t="s">
         <v>87</v>
       </c>
-      <c r="D27" t="s">
+      <c r="G27" t="s">
+        <v>82</v>
+      </c>
+      <c r="L27" t="s">
+        <v>79</v>
+      </c>
+      <c r="M27" t="s">
+        <v>78</v>
+      </c>
+      <c r="N27" t="s">
+        <v>85</v>
+      </c>
+      <c r="O27" t="s">
         <v>84</v>
       </c>
-      <c r="E27" t="s">
-        <v>83</v>
-      </c>
-      <c r="F27" t="s">
-        <v>88</v>
-      </c>
-      <c r="G27" t="s">
-        <v>83</v>
-      </c>
-      <c r="L27" t="s">
-        <v>80</v>
-      </c>
-      <c r="M27" t="s">
+      <c r="P27" t="s">
         <v>79</v>
       </c>
-      <c r="N27" t="s">
-        <v>86</v>
-      </c>
-      <c r="O27" t="s">
-        <v>85</v>
-      </c>
-      <c r="P27" t="s">
-        <v>80</v>
-      </c>
       <c r="Q27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S27" s="2"/>
     </row>
@@ -3923,46 +3923,46 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M28" t="s">
+        <v>78</v>
+      </c>
+      <c r="N28" t="s">
+        <v>85</v>
+      </c>
+      <c r="O28" t="s">
+        <v>84</v>
+      </c>
+      <c r="P28" t="s">
         <v>79</v>
       </c>
-      <c r="N28" t="s">
-        <v>86</v>
-      </c>
-      <c r="O28" t="s">
-        <v>85</v>
-      </c>
-      <c r="P28" t="s">
-        <v>80</v>
-      </c>
       <c r="Q28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S28" s="2"/>
       <c r="T28" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="U28" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="U28" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.3">
@@ -3970,46 +3970,46 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M29" t="s">
+        <v>78</v>
+      </c>
+      <c r="N29" t="s">
+        <v>85</v>
+      </c>
+      <c r="O29" t="s">
+        <v>84</v>
+      </c>
+      <c r="P29" t="s">
         <v>79</v>
       </c>
-      <c r="N29" t="s">
-        <v>86</v>
-      </c>
-      <c r="O29" t="s">
-        <v>85</v>
-      </c>
-      <c r="P29" t="s">
-        <v>80</v>
-      </c>
       <c r="Q29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S29" s="2"/>
       <c r="T29" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="U29" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="U29" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4017,44 +4017,44 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M30" t="s">
+        <v>78</v>
+      </c>
+      <c r="N30" t="s">
+        <v>85</v>
+      </c>
+      <c r="O30" t="s">
+        <v>84</v>
+      </c>
+      <c r="P30" t="s">
         <v>79</v>
       </c>
-      <c r="N30" t="s">
-        <v>86</v>
-      </c>
-      <c r="O30" t="s">
-        <v>85</v>
-      </c>
-      <c r="P30" t="s">
-        <v>80</v>
-      </c>
       <c r="Q30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S30" s="2"/>
       <c r="T30" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="U30" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="U30" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.3">
@@ -4062,46 +4062,46 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M31" t="s">
+        <v>78</v>
+      </c>
+      <c r="N31" t="s">
+        <v>85</v>
+      </c>
+      <c r="O31" t="s">
+        <v>84</v>
+      </c>
+      <c r="P31" t="s">
         <v>79</v>
       </c>
-      <c r="N31" t="s">
-        <v>86</v>
-      </c>
-      <c r="O31" t="s">
-        <v>85</v>
-      </c>
-      <c r="P31" t="s">
-        <v>80</v>
-      </c>
       <c r="Q31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S31" s="2"/>
       <c r="T31" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="U31" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="U31" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.3">
@@ -4109,47 +4109,47 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M32" t="s">
+        <v>78</v>
+      </c>
+      <c r="N32" t="s">
+        <v>85</v>
+      </c>
+      <c r="O32" t="s">
+        <v>84</v>
+      </c>
+      <c r="P32" t="s">
         <v>79</v>
       </c>
-      <c r="N32" t="s">
-        <v>86</v>
-      </c>
-      <c r="O32" t="s">
-        <v>85</v>
-      </c>
-      <c r="P32" t="s">
-        <v>80</v>
-      </c>
       <c r="Q32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S32" s="2"/>
       <c r="T32" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="U32" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="U32" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.3">
@@ -4157,47 +4157,47 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M33" t="s">
+        <v>78</v>
+      </c>
+      <c r="N33" t="s">
+        <v>85</v>
+      </c>
+      <c r="O33" t="s">
+        <v>84</v>
+      </c>
+      <c r="P33" t="s">
         <v>79</v>
       </c>
-      <c r="N33" t="s">
-        <v>86</v>
-      </c>
-      <c r="O33" t="s">
-        <v>85</v>
-      </c>
-      <c r="P33" t="s">
-        <v>80</v>
-      </c>
       <c r="Q33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S33" s="2"/>
       <c r="T33" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="U33" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="U33" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.3">
@@ -4205,47 +4205,47 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M34" t="s">
+        <v>78</v>
+      </c>
+      <c r="N34" t="s">
+        <v>85</v>
+      </c>
+      <c r="O34" t="s">
+        <v>84</v>
+      </c>
+      <c r="P34" t="s">
         <v>79</v>
       </c>
-      <c r="N34" t="s">
-        <v>86</v>
-      </c>
-      <c r="O34" t="s">
-        <v>85</v>
-      </c>
-      <c r="P34" t="s">
-        <v>80</v>
-      </c>
       <c r="Q34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S34" s="2"/>
       <c r="T34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="U34" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="U34" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -4272,13 +4272,13 @@
         <v>34</v>
       </c>
       <c r="C1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s">
         <v>75</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>76</v>
-      </c>
-      <c r="E1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -4289,7 +4289,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -4300,7 +4300,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -4316,7 +4316,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update format and code, fix raw over6
</commit_message>
<xml_diff>
--- a/data/raw_data - Copy.xlsx
+++ b/data/raw_data - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\paktulay-doors\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8673F7E-97E7-4753-B3EF-C459D21BD73F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF2C124-11AC-4632-B1DC-EC04DEE190C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{F3A75742-B43B-409A-9361-00192F1802B9}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="89">
   <si>
     <t>model</t>
   </si>
@@ -265,18 +265,6 @@
     <t>OB4'' + TUTUP M</t>
   </si>
   <si>
-    <t>materi</t>
-  </si>
-  <si>
-    <t>nomor sisi</t>
-  </si>
-  <si>
-    <t>tinggi lebar</t>
-  </si>
-  <si>
-    <t>checked</t>
-  </si>
-  <si>
     <t>AMBANG BAWAH</t>
   </si>
   <si>
@@ -289,31 +277,37 @@
     <t>TIANG MOHER SAMPING</t>
   </si>
   <si>
-    <t>OB4'' + TATAPAN</t>
-  </si>
-  <si>
-    <t>OB4'' + BELL BAWAH</t>
-  </si>
-  <si>
     <t>T SLIDE</t>
   </si>
   <si>
     <t>T KAIT</t>
   </si>
   <si>
-    <t>OB4'' + BELL ATAS</t>
-  </si>
-  <si>
-    <t>OB4'' + TUTUP P</t>
-  </si>
-  <si>
-    <t>M4'' + TATAPAN</t>
-  </si>
-  <si>
-    <t>OB4'' + TUTUP M + BELL BAWAH</t>
-  </si>
-  <si>
     <t>M4'' + TUTUP GOT</t>
+  </si>
+  <si>
+    <t>OB3'' + BELL ATAS</t>
+  </si>
+  <si>
+    <t>OB3'' + TUTUP M + BELL BAWAH</t>
+  </si>
+  <si>
+    <t>OB3'' + BELL BAWAH</t>
+  </si>
+  <si>
+    <t>M3''</t>
+  </si>
+  <si>
+    <t>OB3'' + TATAPAN</t>
+  </si>
+  <si>
+    <t>M3'' + TATAPAN</t>
+  </si>
+  <si>
+    <t>M3'' + TUTUP M</t>
+  </si>
+  <si>
+    <t>OB3'' + TUTUP P</t>
   </si>
 </sst>
 </file>
@@ -335,18 +329,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -367,11 +355,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -689,10 +676,10 @@
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomRight" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1598,7 +1585,8 @@
         <v>39</v>
       </c>
       <c r="C34">
-        <v>6175</v>
+        <f>2042+50</f>
+        <v>2092</v>
       </c>
       <c r="D34">
         <v>2300</v>
@@ -1636,10 +1624,10 @@
   <dimension ref="A1:U34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T29" sqref="T29"/>
+      <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2905,10 +2893,10 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C34" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -2965,10 +2953,10 @@
   <dimension ref="A1:U34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3149,7 +3137,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E6" t="s">
         <v>69</v>
@@ -3164,16 +3152,16 @@
         <v>73</v>
       </c>
       <c r="P6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="Q6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="R6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="S6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -3181,10 +3169,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="G7" t="s">
         <v>69</v>
@@ -3196,16 +3184,16 @@
         <v>73</v>
       </c>
       <c r="P7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="Q7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="R7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="S7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
@@ -3213,10 +3201,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E8" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="G8" t="s">
         <v>69</v>
@@ -3228,16 +3216,16 @@
         <v>73</v>
       </c>
       <c r="P8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="Q8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="R8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="S8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
@@ -3245,13 +3233,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E9" t="s">
         <v>69</v>
       </c>
       <c r="G9" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="M9" t="s">
         <v>71</v>
@@ -3260,16 +3248,16 @@
         <v>73</v>
       </c>
       <c r="P9" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="Q9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="R9" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="S9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
@@ -3277,10 +3265,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E10" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="G10" t="s">
         <v>69</v>
@@ -3292,16 +3280,16 @@
         <v>73</v>
       </c>
       <c r="P10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="Q10" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="R10" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="S10" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
@@ -3309,10 +3297,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E11" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="G11" t="s">
         <v>69</v>
@@ -3324,16 +3312,16 @@
         <v>73</v>
       </c>
       <c r="P11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="Q11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="R11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="S11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
@@ -3341,7 +3329,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E12" t="s">
         <v>69</v>
@@ -3359,16 +3347,16 @@
         <v>73</v>
       </c>
       <c r="P12" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="Q12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="R12" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="S12" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="U12" t="s">
         <v>71</v>
@@ -3379,7 +3367,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E13" t="s">
         <v>69</v>
@@ -3397,16 +3385,16 @@
         <v>73</v>
       </c>
       <c r="P13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="Q13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="R13" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="S13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="U13" t="s">
         <v>71</v>
@@ -3417,10 +3405,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E14" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F14" t="s">
         <v>70</v>
@@ -3435,16 +3423,16 @@
         <v>73</v>
       </c>
       <c r="P14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="Q14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="R14" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="S14" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="U14" t="s">
         <v>71</v>
@@ -3455,10 +3443,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E15" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F15" t="s">
         <v>70</v>
@@ -3473,16 +3461,16 @@
         <v>73</v>
       </c>
       <c r="P15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="Q15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="R15" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="S15" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="U15" t="s">
         <v>71</v>
@@ -3493,328 +3481,344 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D16" t="s">
         <v>83</v>
       </c>
       <c r="E16" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G16" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="L16" t="s">
+        <v>75</v>
+      </c>
+      <c r="M16" t="s">
+        <v>74</v>
+      </c>
+      <c r="N16" t="s">
         <v>79</v>
       </c>
-      <c r="M16" t="s">
+      <c r="O16" t="s">
         <v>78</v>
       </c>
-      <c r="N16" t="s">
-        <v>85</v>
-      </c>
-      <c r="O16" t="s">
-        <v>84</v>
-      </c>
       <c r="P16" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>74</v>
+      </c>
+      <c r="R16" t="s">
+        <v>78</v>
+      </c>
+      <c r="S16" t="s">
         <v>79</v>
       </c>
-      <c r="Q16" t="s">
-        <v>78</v>
-      </c>
-      <c r="R16" t="s">
-        <v>84</v>
-      </c>
-      <c r="S16" s="2"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D17" t="s">
         <v>83</v>
       </c>
       <c r="E17" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G17" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="L17" t="s">
+        <v>75</v>
+      </c>
+      <c r="M17" t="s">
+        <v>74</v>
+      </c>
+      <c r="N17" t="s">
         <v>79</v>
       </c>
-      <c r="M17" t="s">
+      <c r="O17" t="s">
         <v>78</v>
       </c>
-      <c r="N17" t="s">
-        <v>85</v>
-      </c>
-      <c r="O17" t="s">
-        <v>84</v>
-      </c>
       <c r="P17" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>74</v>
+      </c>
+      <c r="R17" t="s">
+        <v>78</v>
+      </c>
+      <c r="S17" t="s">
         <v>79</v>
       </c>
-      <c r="Q17" t="s">
-        <v>78</v>
-      </c>
-      <c r="R17" t="s">
-        <v>84</v>
-      </c>
-      <c r="S17" s="2"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D18" t="s">
         <v>83</v>
       </c>
       <c r="E18" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G18" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="L18" t="s">
+        <v>75</v>
+      </c>
+      <c r="M18" t="s">
+        <v>74</v>
+      </c>
+      <c r="N18" t="s">
         <v>79</v>
       </c>
-      <c r="M18" t="s">
+      <c r="O18" t="s">
         <v>78</v>
       </c>
-      <c r="N18" t="s">
-        <v>85</v>
-      </c>
-      <c r="O18" t="s">
-        <v>84</v>
-      </c>
       <c r="P18" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>74</v>
+      </c>
+      <c r="R18" t="s">
+        <v>78</v>
+      </c>
+      <c r="S18" t="s">
         <v>79</v>
       </c>
-      <c r="Q18" t="s">
-        <v>78</v>
-      </c>
-      <c r="R18" t="s">
-        <v>84</v>
-      </c>
-      <c r="S18" s="2"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D19" t="s">
         <v>83</v>
       </c>
       <c r="E19" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G19" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="L19" t="s">
+        <v>75</v>
+      </c>
+      <c r="M19" t="s">
+        <v>74</v>
+      </c>
+      <c r="N19" t="s">
         <v>79</v>
       </c>
-      <c r="M19" t="s">
+      <c r="O19" t="s">
         <v>78</v>
       </c>
-      <c r="N19" t="s">
-        <v>85</v>
-      </c>
-      <c r="O19" t="s">
-        <v>84</v>
-      </c>
       <c r="P19" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>74</v>
+      </c>
+      <c r="R19" t="s">
+        <v>78</v>
+      </c>
+      <c r="S19" t="s">
         <v>79</v>
       </c>
-      <c r="Q19" t="s">
-        <v>78</v>
-      </c>
-      <c r="R19" t="s">
-        <v>84</v>
-      </c>
-      <c r="S19" s="2"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D20" t="s">
         <v>83</v>
       </c>
       <c r="E20" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G20" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="L20" t="s">
+        <v>75</v>
+      </c>
+      <c r="M20" t="s">
+        <v>74</v>
+      </c>
+      <c r="N20" t="s">
         <v>79</v>
       </c>
-      <c r="M20" t="s">
+      <c r="O20" t="s">
         <v>78</v>
       </c>
-      <c r="N20" t="s">
-        <v>85</v>
-      </c>
-      <c r="O20" t="s">
-        <v>84</v>
-      </c>
       <c r="P20" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>74</v>
+      </c>
+      <c r="R20" t="s">
+        <v>78</v>
+      </c>
+      <c r="S20" t="s">
         <v>79</v>
       </c>
-      <c r="Q20" t="s">
-        <v>78</v>
-      </c>
-      <c r="R20" t="s">
-        <v>84</v>
-      </c>
-      <c r="S20" s="2"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D21" t="s">
         <v>83</v>
       </c>
       <c r="E21" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G21" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="L21" t="s">
+        <v>75</v>
+      </c>
+      <c r="M21" t="s">
+        <v>74</v>
+      </c>
+      <c r="N21" t="s">
         <v>79</v>
       </c>
-      <c r="M21" t="s">
+      <c r="O21" t="s">
         <v>78</v>
       </c>
-      <c r="N21" t="s">
-        <v>85</v>
-      </c>
-      <c r="O21" t="s">
-        <v>84</v>
-      </c>
       <c r="P21" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>74</v>
+      </c>
+      <c r="R21" t="s">
+        <v>78</v>
+      </c>
+      <c r="S21" t="s">
         <v>79</v>
       </c>
-      <c r="Q21" t="s">
-        <v>78</v>
-      </c>
-      <c r="R21" t="s">
-        <v>84</v>
-      </c>
-      <c r="S21" s="2"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D22" t="s">
         <v>83</v>
       </c>
       <c r="E22" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G22" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="L22" t="s">
+        <v>75</v>
+      </c>
+      <c r="M22" t="s">
+        <v>74</v>
+      </c>
+      <c r="N22" t="s">
         <v>79</v>
       </c>
-      <c r="M22" t="s">
+      <c r="O22" t="s">
         <v>78</v>
       </c>
-      <c r="N22" t="s">
-        <v>85</v>
-      </c>
-      <c r="O22" t="s">
-        <v>84</v>
-      </c>
       <c r="P22" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>74</v>
+      </c>
+      <c r="R22" t="s">
+        <v>78</v>
+      </c>
+      <c r="S22" t="s">
         <v>79</v>
       </c>
-      <c r="Q22" t="s">
-        <v>78</v>
-      </c>
-      <c r="R22" t="s">
-        <v>84</v>
-      </c>
-      <c r="S22" s="2"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D23" t="s">
         <v>83</v>
       </c>
       <c r="E23" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G23" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="L23" t="s">
+        <v>75</v>
+      </c>
+      <c r="M23" t="s">
+        <v>74</v>
+      </c>
+      <c r="N23" t="s">
         <v>79</v>
       </c>
-      <c r="M23" t="s">
+      <c r="O23" t="s">
         <v>78</v>
       </c>
-      <c r="N23" t="s">
-        <v>85</v>
-      </c>
-      <c r="O23" t="s">
-        <v>84</v>
-      </c>
       <c r="P23" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>74</v>
+      </c>
+      <c r="R23" t="s">
+        <v>78</v>
+      </c>
+      <c r="S23" t="s">
         <v>79</v>
       </c>
-      <c r="Q23" t="s">
-        <v>78</v>
-      </c>
-      <c r="R23" t="s">
-        <v>84</v>
-      </c>
-      <c r="S23" s="2"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="D24" t="s">
         <v>71</v>
       </c>
       <c r="E24" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="G24" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
@@ -3822,16 +3826,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="D25" t="s">
         <v>71</v>
       </c>
       <c r="E25" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="G25" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.3">
@@ -3839,127 +3843,133 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D26" t="s">
         <v>83</v>
       </c>
       <c r="E26" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G26" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="L26" t="s">
+        <v>75</v>
+      </c>
+      <c r="M26" t="s">
+        <v>74</v>
+      </c>
+      <c r="N26" t="s">
         <v>79</v>
       </c>
-      <c r="M26" t="s">
+      <c r="O26" t="s">
         <v>78</v>
       </c>
-      <c r="N26" t="s">
-        <v>85</v>
-      </c>
-      <c r="O26" t="s">
-        <v>84</v>
-      </c>
       <c r="P26" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>74</v>
+      </c>
+      <c r="R26" t="s">
+        <v>78</v>
+      </c>
+      <c r="S26" t="s">
         <v>79</v>
       </c>
-      <c r="Q26" t="s">
-        <v>78</v>
-      </c>
-      <c r="R26" t="s">
-        <v>84</v>
-      </c>
-      <c r="S26" s="2"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D27" t="s">
         <v>83</v>
       </c>
       <c r="E27" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F27" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G27" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="L27" t="s">
+        <v>75</v>
+      </c>
+      <c r="M27" t="s">
+        <v>74</v>
+      </c>
+      <c r="N27" t="s">
         <v>79</v>
       </c>
-      <c r="M27" t="s">
+      <c r="O27" t="s">
         <v>78</v>
       </c>
-      <c r="N27" t="s">
-        <v>85</v>
-      </c>
-      <c r="O27" t="s">
-        <v>84</v>
-      </c>
       <c r="P27" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>74</v>
+      </c>
+      <c r="R27" t="s">
+        <v>78</v>
+      </c>
+      <c r="S27" t="s">
         <v>79</v>
       </c>
-      <c r="Q27" t="s">
-        <v>78</v>
-      </c>
-      <c r="R27" t="s">
-        <v>84</v>
-      </c>
-      <c r="S27" s="2"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>86</v>
+      <c r="B28" t="s">
+        <v>81</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L28" t="s">
+        <v>75</v>
+      </c>
+      <c r="M28" t="s">
+        <v>74</v>
+      </c>
+      <c r="N28" t="s">
         <v>79</v>
       </c>
-      <c r="M28" t="s">
+      <c r="O28" t="s">
         <v>78</v>
       </c>
-      <c r="N28" t="s">
-        <v>85</v>
-      </c>
-      <c r="O28" t="s">
-        <v>84</v>
-      </c>
       <c r="P28" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>74</v>
+      </c>
+      <c r="R28" t="s">
+        <v>78</v>
+      </c>
+      <c r="S28" t="s">
         <v>79</v>
       </c>
-      <c r="Q28" t="s">
-        <v>78</v>
-      </c>
-      <c r="R28" t="s">
-        <v>84</v>
-      </c>
-      <c r="S28" s="2"/>
       <c r="T28" s="1" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="U28" s="1" t="s">
         <v>71</v>
@@ -3969,44 +3979,46 @@
       <c r="A29" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>86</v>
+      <c r="B29" t="s">
+        <v>81</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L29" t="s">
+        <v>75</v>
+      </c>
+      <c r="M29" t="s">
+        <v>74</v>
+      </c>
+      <c r="N29" t="s">
         <v>79</v>
       </c>
-      <c r="M29" t="s">
+      <c r="O29" t="s">
         <v>78</v>
       </c>
-      <c r="N29" t="s">
-        <v>85</v>
-      </c>
-      <c r="O29" t="s">
-        <v>84</v>
-      </c>
       <c r="P29" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>74</v>
+      </c>
+      <c r="R29" t="s">
+        <v>78</v>
+      </c>
+      <c r="S29" t="s">
         <v>79</v>
       </c>
-      <c r="Q29" t="s">
-        <v>78</v>
-      </c>
-      <c r="R29" t="s">
-        <v>84</v>
-      </c>
-      <c r="S29" s="2"/>
       <c r="T29" s="1" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="U29" s="1" t="s">
         <v>71</v>
@@ -4016,42 +4028,44 @@
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="G30" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L30" t="s">
+        <v>75</v>
+      </c>
+      <c r="M30" t="s">
+        <v>74</v>
+      </c>
+      <c r="N30" t="s">
         <v>79</v>
       </c>
-      <c r="M30" t="s">
+      <c r="O30" t="s">
         <v>78</v>
       </c>
-      <c r="N30" t="s">
-        <v>85</v>
-      </c>
-      <c r="O30" t="s">
-        <v>84</v>
-      </c>
       <c r="P30" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>74</v>
+      </c>
+      <c r="R30" t="s">
+        <v>78</v>
+      </c>
+      <c r="S30" t="s">
         <v>79</v>
       </c>
-      <c r="Q30" t="s">
-        <v>78</v>
-      </c>
-      <c r="R30" t="s">
-        <v>84</v>
-      </c>
-      <c r="S30" s="2"/>
       <c r="T30" s="1" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="U30" s="1" t="s">
         <v>71</v>
@@ -4061,44 +4075,46 @@
       <c r="A31" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>86</v>
+      <c r="B31" t="s">
+        <v>81</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L31" t="s">
+        <v>75</v>
+      </c>
+      <c r="M31" t="s">
+        <v>74</v>
+      </c>
+      <c r="N31" t="s">
         <v>79</v>
       </c>
-      <c r="M31" t="s">
+      <c r="O31" t="s">
         <v>78</v>
       </c>
-      <c r="N31" t="s">
-        <v>85</v>
-      </c>
-      <c r="O31" t="s">
-        <v>84</v>
-      </c>
       <c r="P31" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>74</v>
+      </c>
+      <c r="R31" t="s">
+        <v>78</v>
+      </c>
+      <c r="S31" t="s">
         <v>79</v>
       </c>
-      <c r="Q31" t="s">
-        <v>78</v>
-      </c>
-      <c r="R31" t="s">
-        <v>84</v>
-      </c>
-      <c r="S31" s="2"/>
       <c r="T31" s="1" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="U31" s="1" t="s">
         <v>71</v>
@@ -4108,45 +4124,47 @@
       <c r="A32" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>70</v>
+      <c r="F32" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L32" t="s">
+        <v>75</v>
+      </c>
+      <c r="M32" t="s">
+        <v>74</v>
+      </c>
+      <c r="N32" t="s">
         <v>79</v>
       </c>
-      <c r="M32" t="s">
+      <c r="O32" t="s">
         <v>78</v>
       </c>
-      <c r="N32" t="s">
-        <v>85</v>
-      </c>
-      <c r="O32" t="s">
-        <v>84</v>
-      </c>
       <c r="P32" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>74</v>
+      </c>
+      <c r="R32" t="s">
+        <v>78</v>
+      </c>
+      <c r="S32" t="s">
         <v>79</v>
       </c>
-      <c r="Q32" t="s">
-        <v>78</v>
-      </c>
-      <c r="R32" t="s">
-        <v>84</v>
-      </c>
-      <c r="S32" s="2"/>
       <c r="T32" s="1" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="U32" s="1" t="s">
         <v>71</v>
@@ -4156,45 +4174,47 @@
       <c r="A33" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>70</v>
+      <c r="F33" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L33" t="s">
+        <v>75</v>
+      </c>
+      <c r="M33" t="s">
+        <v>74</v>
+      </c>
+      <c r="N33" t="s">
         <v>79</v>
       </c>
-      <c r="M33" t="s">
+      <c r="O33" t="s">
         <v>78</v>
       </c>
-      <c r="N33" t="s">
-        <v>85</v>
-      </c>
-      <c r="O33" t="s">
-        <v>84</v>
-      </c>
       <c r="P33" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>74</v>
+      </c>
+      <c r="R33" t="s">
+        <v>78</v>
+      </c>
+      <c r="S33" t="s">
         <v>79</v>
       </c>
-      <c r="Q33" t="s">
-        <v>78</v>
-      </c>
-      <c r="R33" t="s">
-        <v>84</v>
-      </c>
-      <c r="S33" s="2"/>
       <c r="T33" s="1" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="U33" s="1" t="s">
         <v>71</v>
@@ -4204,45 +4224,47 @@
       <c r="A34" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>70</v>
+      <c r="F34" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L34" t="s">
+        <v>75</v>
+      </c>
+      <c r="M34" t="s">
+        <v>74</v>
+      </c>
+      <c r="N34" t="s">
         <v>79</v>
       </c>
-      <c r="M34" t="s">
+      <c r="O34" t="s">
         <v>78</v>
       </c>
-      <c r="N34" t="s">
-        <v>85</v>
-      </c>
-      <c r="O34" t="s">
-        <v>84</v>
-      </c>
       <c r="P34" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>74</v>
+      </c>
+      <c r="R34" t="s">
+        <v>78</v>
+      </c>
+      <c r="S34" t="s">
         <v>79</v>
       </c>
-      <c r="Q34" t="s">
-        <v>78</v>
-      </c>
-      <c r="R34" t="s">
-        <v>84</v>
-      </c>
-      <c r="S34" s="2"/>
       <c r="T34" s="1" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="U34" s="1" t="s">
         <v>71</v>
@@ -4256,70 +4278,52 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14EBC57D-6317-4B50-8B05-B06366025BD0}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C1" sqref="C1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -4327,7 +4331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -4335,7 +4339,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -4343,7 +4347,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -4351,7 +4355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -4359,7 +4363,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -4367,7 +4371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -4375,7 +4379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -4383,7 +4387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -4391,7 +4395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -4399,7 +4403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>

</xml_diff>